<commit_message>
add 1275 and 506
</commit_message>
<xml_diff>
--- a/array_string/record.xlsx
+++ b/array_string/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\someIdeaPrac\leetcode\array_string\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4EE2D0-28F8-4EE7-83ED-E419E2BD1063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A473C0-74A6-46BB-9164-6CCF6AEE6831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>题号</t>
   </si>
@@ -80,6 +80,26 @@
   </si>
   <si>
     <t>以为自己做的很麻烦，实际上看了题解发现都是这么做的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1275找出井字棋的获胜者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过位运算非常优雅地解决了，记录一下，有空更新自己的做法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>506相对名次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两种方法，一种通过哈希表，另一种实现过程中用到了lambda表达式排序，故记录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -487,6 +507,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>